<commit_message>
correction finish avec dao
</commit_message>
<xml_diff>
--- a/BaremeJavaBaseTest1_KL16.xlsx
+++ b/BaremeJavaBaseTest1_KL16.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F9708C-92C7-4F1D-9EA8-1A8E3E01BF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCC546F-3DF2-46DA-AED7-09FE11C3324D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18375" yWindow="510" windowWidth="12600" windowHeight="10515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -3755,11 +3755,11 @@
   <dimension ref="A1:BT97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2205" ySplit="3975" topLeftCell="AX8" activePane="topRight"/>
+      <pane xSplit="2205" ySplit="3975" topLeftCell="G8" activePane="bottomRight"/>
       <selection activeCell="B1" sqref="B1:C1048576"/>
       <selection pane="topRight" activeCell="BI5" sqref="BI5"/>
       <selection pane="bottomLeft" activeCell="A26" sqref="A26:XFD26"/>
-      <selection pane="bottomRight" activeCell="BI27" sqref="BI27"/>
+      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -7757,7 +7757,9 @@
       <c r="J22" s="49">
         <v>99</v>
       </c>
-      <c r="K22" s="59"/>
+      <c r="K22" s="59">
+        <v>0</v>
+      </c>
       <c r="L22" s="49">
         <v>99</v>
       </c>
@@ -9526,7 +9528,7 @@
       </c>
       <c r="K33" s="58">
         <f>AVERAGE(K8:K27)</f>
-        <v>0.34027777777777779</v>
+        <v>0.32236842105263158</v>
       </c>
       <c r="L33" s="89">
         <f>AVERAGE(L8:L24)</f>

</xml_diff>